<commit_message>
add client and property permission
</commit_message>
<xml_diff>
--- a/TradesMate/Book1.xlsx
+++ b/TradesMate/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Porjects\TradesMateV2\TradesMate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tutorial\TradesMateV2\TradesMate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Company</t>
   </si>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,6 +217,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -252,6 +269,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,19 +441,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G2" t="s">
         <v>13</v>
       </c>
@@ -444,7 +478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -461,10 +495,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
@@ -472,17 +509,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -493,7 +530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -501,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
add new entities test working
</commit_message>
<xml_diff>
--- a/TradesMate/Book1.xlsx
+++ b/TradesMate/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tutorial\TradesMateV2\TradesMate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Porjects\TradesMateV2\TradesMate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Company</t>
   </si>
@@ -50,21 +50,12 @@
     <t>User(Trade People)</t>
   </si>
   <si>
-    <t>Roger Yearwood</t>
-  </si>
-  <si>
-    <t>Ralph Carrow</t>
-  </si>
-  <si>
     <t>Oleg Lien(Admin)</t>
   </si>
   <si>
     <t>Billy Bomen (Admin)</t>
   </si>
   <si>
-    <t>Elwood Olin</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
@@ -87,12 +78,42 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Roger Yearwood(Default)</t>
+  </si>
+  <si>
+    <t>Ralph Carrow Default)</t>
+  </si>
+  <si>
+    <t>Elwood Olin Default)</t>
+  </si>
+  <si>
+    <t>Sonny Getchell (Contractor)</t>
+  </si>
+  <si>
+    <t>Taylor Diniz((Contractor))</t>
+  </si>
+  <si>
+    <t>Simon's Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonny's Allocation: Simon's </t>
+  </si>
+  <si>
+    <t>Share same property as Lee</t>
+  </si>
+  <si>
+    <t>Taylor's Allocation: Lee's</t>
+  </si>
+  <si>
+    <t>Taylor's Allocation: Joe's</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,23 +238,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -269,23 +273,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,22 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,21 +451,21 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -489,13 +476,13 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -503,44 +490,79 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>